<commit_message>
datasett låst for price sensitivity pulp
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT_pulp.xlsx
+++ b/Input_data_With_dummyGrid_and_RT_pulp.xlsx
@@ -5,52 +5,48 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\V8\Master_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Price_sensitivity\Price_sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE35D3F4-1EA4-478C-984C-EF3E9D8BC619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96B8402-B88A-4249-99F7-50DCC0CBEE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
     <sheet name="Par_CarbonIntensity" sheetId="9" r:id="rId2"/>
-    <sheet name="Par_CostEmission_1_2025" sheetId="11" r:id="rId3"/>
-    <sheet name="Par_CostEmission_1_2050" sheetId="75" r:id="rId4"/>
-    <sheet name="Par_CostEmission_2_2025" sheetId="76" r:id="rId5"/>
-    <sheet name="Par_CostEmission_2_2050" sheetId="77" r:id="rId6"/>
-    <sheet name="Par_CostEmission_3_2025" sheetId="78" r:id="rId7"/>
-    <sheet name="Par_CostEmission_3_2050" sheetId="79" r:id="rId8"/>
-    <sheet name="Par_CostEmission_4_2025" sheetId="80" r:id="rId9"/>
-    <sheet name="Par_CostEmission_4_2050" sheetId="81" r:id="rId10"/>
-    <sheet name="Par_CostEmission_5_2025" sheetId="82" r:id="rId11"/>
-    <sheet name="Par_CostEmission_5_2050" sheetId="83" r:id="rId12"/>
-    <sheet name="Par_Power2Energy_ratio" sheetId="45" r:id="rId13"/>
-    <sheet name="Par_ChargeEfficiency" sheetId="10" r:id="rId14"/>
-    <sheet name="Par_DischargeEfficiency" sheetId="14" r:id="rId15"/>
-    <sheet name="Par_ECToTech_Efficiency" sheetId="15" r:id="rId16"/>
-    <sheet name="Par_TechToEC_Efficiency" sheetId="29" r:id="rId17"/>
-    <sheet name="Par_InitialCapacityInstalled" sheetId="19" r:id="rId18"/>
-    <sheet name="Par_InitialSoC" sheetId="20" r:id="rId19"/>
-    <sheet name="Par_MaxChargeDischargeRate" sheetId="22" r:id="rId20"/>
-    <sheet name="Par_MaxStorageCapacity" sheetId="25" r:id="rId21"/>
-    <sheet name="Par_MaxExport" sheetId="24" r:id="rId22"/>
-    <sheet name="Par_SelfDischarge" sheetId="28" r:id="rId23"/>
-    <sheet name="Set_of_EnergyCarrier" sheetId="30" r:id="rId24"/>
-    <sheet name="Set_of_FlexibleLoad" sheetId="31" r:id="rId25"/>
-    <sheet name="Set_of_FlexibleLoadForEC" sheetId="32" r:id="rId26"/>
-    <sheet name="Set_of_Month" sheetId="33" r:id="rId27"/>
-    <sheet name="Par_Ramping_factor" sheetId="64" r:id="rId28"/>
-    <sheet name="Set_of_Technology" sheetId="35" r:id="rId29"/>
-    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId30"/>
-    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId31"/>
-    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId32"/>
-    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId33"/>
-    <sheet name="Par_Cost_LS" sheetId="74" r:id="rId34"/>
-    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId35"/>
-    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId36"/>
-    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId37"/>
-    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId38"/>
+    <sheet name="Par_CostEmission_exp_2025" sheetId="11" r:id="rId3"/>
+    <sheet name="Par_CostEmission_exp_2050" sheetId="75" r:id="rId4"/>
+    <sheet name="Par_CostEmission_high_2025" sheetId="76" r:id="rId5"/>
+    <sheet name="Par_CostEmission_high_2050" sheetId="77" r:id="rId6"/>
+    <sheet name="Par_CostEmission_low_2025" sheetId="78" r:id="rId7"/>
+    <sheet name="Par_CostEmission_low_2050" sheetId="79" r:id="rId8"/>
+    <sheet name="Par_Power2Energy_ratio" sheetId="45" r:id="rId9"/>
+    <sheet name="Par_ChargeEfficiency" sheetId="10" r:id="rId10"/>
+    <sheet name="Par_DischargeEfficiency" sheetId="14" r:id="rId11"/>
+    <sheet name="Par_ECToTech_Efficiency" sheetId="15" r:id="rId12"/>
+    <sheet name="Par_TechToEC_Efficiency" sheetId="29" r:id="rId13"/>
+    <sheet name="Par_InitialCapacityInstalled" sheetId="19" r:id="rId14"/>
+    <sheet name="Par_InitialSoC" sheetId="20" r:id="rId15"/>
+    <sheet name="Par_MaxChargeDischargeRate" sheetId="22" r:id="rId16"/>
+    <sheet name="Par_MaxStorageCapacity" sheetId="25" r:id="rId17"/>
+    <sheet name="Par_MaxExport" sheetId="24" r:id="rId18"/>
+    <sheet name="Par_SelfDischarge" sheetId="28" r:id="rId19"/>
+    <sheet name="Set_of_EnergyCarrier" sheetId="30" r:id="rId20"/>
+    <sheet name="Set_of_FlexibleLoad" sheetId="31" r:id="rId21"/>
+    <sheet name="Set_of_FlexibleLoadForEC" sheetId="32" r:id="rId22"/>
+    <sheet name="Set_of_Month" sheetId="33" r:id="rId23"/>
+    <sheet name="Par_Ramping_factor" sheetId="64" r:id="rId24"/>
+    <sheet name="Set_of_Technology" sheetId="35" r:id="rId25"/>
+    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId26"/>
+    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId27"/>
+    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId28"/>
+    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId29"/>
+    <sheet name="Par_Cost_LS" sheetId="74" r:id="rId30"/>
+    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId31"/>
+    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId32"/>
+    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId33"/>
+    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -226,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="87">
   <si>
     <t>Benevning:</t>
   </si>
@@ -1206,208 +1202,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A51869F-FCE4-4F4E-BC22-A2772323E192}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>0.77683760700000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21444BD-96C7-41C5-8C58-840EC3753E8F}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>5.2051281999999997E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4745B9-33CD-4F54-B24F-2FB1EF9BEFBD}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>0.124786325</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65669FF3-9BA1-4500-B472-59EFCF72B795}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <f>0.5/2</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <f>300/3000</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <f>2.9/175</f>
-        <v>1.657142857142857E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <f>0.1/16.7</f>
-        <v>5.9880239520958087E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1504,7 +1298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1597,11 +1391,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +1993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
@@ -3037,7 +2831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -3231,7 +3025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3323,6 +3117,331 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>130000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <f>0.001/24</f>
+        <v>4.1666666666666665E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>0.03/24</f>
+        <v>1.25E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <f>0.002/24</f>
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f>0.01/24</f>
+        <v>4.1666666666666669E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3948,331 +4067,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>130000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <f>0.001/24</f>
-        <v>4.1666666666666665E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <f>0.03/24</f>
-        <v>1.25E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <f>0.002/24</f>
-        <v>8.3333333333333331E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <f>0.01/24</f>
-        <v>4.1666666666666669E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A3:A11"/>
   <sheetViews>
@@ -4335,7 +4129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A3:A10"/>
   <sheetViews>
@@ -4393,7 +4187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -4476,7 +4270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -4501,7 +4295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC2358-B737-4B12-BCF2-983233884487}">
   <dimension ref="A3:B20"/>
   <sheetViews>
@@ -4664,7 +4458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A3:D25"/>
   <sheetViews>
@@ -4791,6 +4585,1264 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+  <dimension ref="A3:C55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+  <dimension ref="A3:F78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
+  <dimension ref="A3:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y32" sqref="Y32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815BD0D-D4C8-43C3-B5E1-419A131BCC6A}">
+  <dimension ref="A2:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2.6160000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4834,1264 +5886,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
-  <dimension ref="A3:C55"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A3:F78"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>75</v>
-      </c>
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F78" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
-  <dimension ref="A3:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815BD0D-D4C8-43C3-B5E1-419A131BCC6A}">
-  <dimension ref="A2:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0.95699999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>2.6160000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
   <dimension ref="A3:B11"/>
   <sheetViews>
@@ -6181,7 +5975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
   <dimension ref="A3:B20"/>
   <sheetViews>
@@ -6343,7 +6137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -6425,7 +6219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB31CFC9-E7A6-4B4A-99A3-E708E722ECEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -6453,7 +6247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -6625,8 +6419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7705B9F7-B1BE-45C3-99A7-E4CE7496911B}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6657,33 +6451,95 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1862DBF7-FCD8-4BA0-B9A8-61126D38663C}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65669FF3-9BA1-4500-B472-59EFCF72B795}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>0.18333333299999999</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>0.5/2</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f>300/3000</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <f>2.9/175</f>
+        <v>1.657142857142857E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f>0.1/16.7</f>
+        <v>5.9880239520958087E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6692,6 +6548,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6892,41 +6768,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6949,9 +6794,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>